<commit_message>
Final working version using Excel upload
</commit_message>
<xml_diff>
--- a/Glassline Damage Report.xlsx
+++ b/Glassline Damage Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F130FA53-496B-4D1B-B9CC-E27D46C1DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD60E7B-2727-4E2C-AB2B-F121EE038C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1252,7 +1252,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1277,6 +1276,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1344,17 +1344,17 @@
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Date" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Month" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year" dataDxfId="8">
       <calculatedColumnFormula>YEAR(RejectionData[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Size" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Thickness (mm)" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Type" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Reason" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Qty" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Vendor" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="SO" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Dept." dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Size" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Thickness (mm)" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Type" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Reason" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Qty" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Vendor" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="SO" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Dept." dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1649,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B26" sqref="B25:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>